<commit_message>
DGTL-107:Done Login Page TestCases
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelSheet/LoginCredentials.xlsx
+++ b/src/test/resources/ExcelSheet/LoginCredentials.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="Email" sheetId="2" r:id="rId2"/>
+    <sheet name="New Customer" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>mngr472520</t>
   </si>
@@ -29,6 +30,69 @@
   </si>
   <si>
     <t>ainapur@gmail.com</t>
+  </si>
+  <si>
+    <t>Customer Name</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Date Of Birth</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">City </t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>PIN</t>
+  </si>
+  <si>
+    <t>Tel. No</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Rajesh Kumar</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Hno-104,Street no.2</t>
+  </si>
+  <si>
+    <t>Mumbai</t>
+  </si>
+  <si>
+    <t>Maharashtra</t>
+  </si>
+  <si>
+    <t>rkumar12@sdhaj.com</t>
+  </si>
+  <si>
+    <t>Saniya Patel</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Fl.A-405, Lane2</t>
+  </si>
+  <si>
+    <t>Pune</t>
+  </si>
+  <si>
+    <t>sanpatel@asa.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
   </si>
 </sst>
 </file>
@@ -73,9 +137,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -357,10 +422,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -377,6 +442,14 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -386,8 +459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -403,4 +476,112 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="2">
+        <v>33531</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2">
+        <v>400001</v>
+      </c>
+      <c r="H2">
+        <v>23452472348</v>
+      </c>
+      <c r="I2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="2">
+        <v>34227</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3">
+        <v>416532</v>
+      </c>
+      <c r="H3">
+        <v>234587912</v>
+      </c>
+      <c r="I3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
DGTL-108:Done Listeners , Generated Extent Report
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelSheet/LoginCredentials.xlsx
+++ b/src/test/resources/ExcelSheet/LoginCredentials.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -459,7 +459,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
@@ -482,8 +482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -491,7 +491,10 @@
     <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>